<commit_message>
Updated time column in raw WR data
</commit_message>
<xml_diff>
--- a/data/raw/running_world_record_data.xlsx
+++ b/data/raw/running_world_record_data.xlsx
@@ -1,9 +1,9 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="25213"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="25217"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{908585B3-51B6-4599-A16C-09499852D5D0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{5213F6D8-9870-4452-8E7B-C16BB758DA9C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="19">
   <si>
     <t>Distance</t>
   </si>
@@ -45,6 +45,18 @@
   </si>
   <si>
     <t>Height</t>
+  </si>
+  <si>
+    <t>[m]</t>
+  </si>
+  <si>
+    <t>[s]</t>
+  </si>
+  <si>
+    <t>[-]</t>
+  </si>
+  <si>
+    <t>[kg]</t>
   </si>
   <si>
     <t>Usain Bolt</t>
@@ -426,10 +438,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F14"/>
+  <dimension ref="A1:G15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B14" sqref="B14"/>
+      <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -439,7 +451,7 @@
     <col min="7" max="7" width="12.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6">
+    <row r="1" spans="1:7">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -459,248 +471,289 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:6">
-      <c r="A2">
+    <row r="2" spans="1:7">
+      <c r="A2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C2" t="s">
+        <v>8</v>
+      </c>
+      <c r="D2" t="s">
+        <v>8</v>
+      </c>
+      <c r="E2" t="s">
+        <v>9</v>
+      </c>
+      <c r="F2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7">
+      <c r="A3">
         <v>100</v>
       </c>
-      <c r="B2" s="1">
-        <v>1.1087962962962965E-4</v>
-      </c>
-      <c r="C2">
-        <v>2009</v>
-      </c>
-      <c r="D2" t="s">
-        <v>6</v>
-      </c>
-      <c r="E2">
-        <v>86</v>
-      </c>
-      <c r="F2">
-        <v>195</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6">
-      <c r="A3">
-        <v>200</v>
-      </c>
-      <c r="B3" s="1">
-        <v>2.2210648148148152E-4</v>
+      <c r="B3">
+        <v>9.6</v>
       </c>
       <c r="C3">
         <v>2009</v>
       </c>
       <c r="D3" t="s">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="E3">
         <v>86</v>
       </c>
       <c r="F3">
-        <v>195</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6">
+        <v>1.95</v>
+      </c>
+      <c r="G3" s="1"/>
+    </row>
+    <row r="4" spans="1:7">
       <c r="A4">
+        <v>200</v>
+      </c>
+      <c r="B4">
+        <v>19.2</v>
+      </c>
+      <c r="C4">
+        <v>2009</v>
+      </c>
+      <c r="D4" t="s">
+        <v>10</v>
+      </c>
+      <c r="E4">
+        <v>86</v>
+      </c>
+      <c r="F4">
+        <v>1.95</v>
+      </c>
+      <c r="G4" s="1"/>
+    </row>
+    <row r="5" spans="1:7">
+      <c r="A5">
         <v>400</v>
       </c>
-      <c r="B4" s="1">
-        <v>4.9803240740740743E-4</v>
-      </c>
-      <c r="C4">
+      <c r="B5">
+        <v>43</v>
+      </c>
+      <c r="C5">
         <v>2016</v>
       </c>
-      <c r="D4" t="s">
-        <v>7</v>
-      </c>
-      <c r="E4">
+      <c r="D5" t="s">
+        <v>11</v>
+      </c>
+      <c r="E5">
         <v>70</v>
       </c>
-      <c r="F4">
-        <v>183</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6">
-      <c r="A5">
+      <c r="F5">
+        <v>1.83</v>
+      </c>
+      <c r="G5" s="1"/>
+    </row>
+    <row r="6" spans="1:7">
+      <c r="A6">
         <v>800</v>
       </c>
-      <c r="B5" s="1">
-        <v>1.1689814814814816E-3</v>
-      </c>
-      <c r="C5">
+      <c r="B6">
+        <f>60+41</f>
+        <v>101</v>
+      </c>
+      <c r="C6">
         <v>2012</v>
       </c>
-      <c r="D5" t="s">
-        <v>8</v>
-      </c>
-      <c r="E5">
+      <c r="D6" t="s">
+        <v>12</v>
+      </c>
+      <c r="E6">
         <v>76</v>
       </c>
-      <c r="F5">
-        <v>190</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6">
-      <c r="A6">
+      <c r="F6">
+        <v>1.9</v>
+      </c>
+      <c r="G6" s="1"/>
+    </row>
+    <row r="7" spans="1:7">
+      <c r="A7">
         <v>1000</v>
       </c>
-      <c r="B6" s="1">
-        <v>1.5273148148148147E-3</v>
-      </c>
-      <c r="C6">
+      <c r="B7">
+        <f>2*60+12</f>
+        <v>132</v>
+      </c>
+      <c r="C7">
         <v>1999</v>
       </c>
-      <c r="D6" t="s">
-        <v>9</v>
-      </c>
-      <c r="E6">
+      <c r="D7" t="s">
+        <v>13</v>
+      </c>
+      <c r="E7">
         <v>68</v>
       </c>
-      <c r="F6">
-        <v>182</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6">
-      <c r="A7">
+      <c r="F7">
+        <v>1.82</v>
+      </c>
+      <c r="G7" s="1"/>
+    </row>
+    <row r="8" spans="1:7">
+      <c r="A8">
         <v>1500</v>
       </c>
-      <c r="B7" s="1">
-        <v>2.3842592592592591E-3</v>
-      </c>
-      <c r="C7">
+      <c r="B8">
+        <f>3*60+26</f>
+        <v>206</v>
+      </c>
+      <c r="C8">
         <v>1998</v>
       </c>
-      <c r="D7" t="s">
-        <v>10</v>
-      </c>
-      <c r="E7">
-        <v>58</v>
-      </c>
-      <c r="F7">
-        <v>176</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6">
-      <c r="A8">
-        <v>2000</v>
-      </c>
-      <c r="B8" s="1">
-        <v>3.2961805555555557E-3</v>
-      </c>
-      <c r="C8">
-        <v>1999</v>
-      </c>
       <c r="D8" t="s">
-        <v>10</v>
+        <v>14</v>
       </c>
       <c r="E8">
         <v>58</v>
       </c>
       <c r="F8">
-        <v>176</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6">
+        <v>1.76</v>
+      </c>
+      <c r="G8" s="1"/>
+    </row>
+    <row r="9" spans="1:7">
       <c r="A9">
+        <v>2000</v>
+      </c>
+      <c r="B9">
+        <f>4*60+44.8</f>
+        <v>284.8</v>
+      </c>
+      <c r="C9">
+        <v>1999</v>
+      </c>
+      <c r="D9" t="s">
+        <v>14</v>
+      </c>
+      <c r="E9">
+        <v>58</v>
+      </c>
+      <c r="F9">
+        <v>1.76</v>
+      </c>
+      <c r="G9" s="1"/>
+    </row>
+    <row r="10" spans="1:7">
+      <c r="A10">
         <v>3000</v>
       </c>
-      <c r="B9" s="1">
-        <v>5.1003472222222223E-3</v>
-      </c>
-      <c r="C9">
+      <c r="B10">
+        <f>7*60+20.7</f>
+        <v>440.7</v>
+      </c>
+      <c r="C10">
         <v>1996</v>
       </c>
-      <c r="D9" t="s">
-        <v>11</v>
-      </c>
-      <c r="E9">
+      <c r="D10" t="s">
+        <v>15</v>
+      </c>
+      <c r="E10">
         <v>55</v>
       </c>
-      <c r="F9">
-        <v>170</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6">
-      <c r="A10">
+      <c r="F10">
+        <v>1.7</v>
+      </c>
+      <c r="G10" s="1"/>
+    </row>
+    <row r="11" spans="1:7">
+      <c r="A11">
         <v>5000</v>
       </c>
-      <c r="B10" s="1">
-        <v>8.7425925925925935E-3</v>
-      </c>
-      <c r="C10">
-        <v>2020</v>
-      </c>
-      <c r="D10" t="s">
-        <v>12</v>
-      </c>
-      <c r="E10">
-        <v>52</v>
-      </c>
-      <c r="F10">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6">
-      <c r="A11">
-        <v>10000</v>
-      </c>
-      <c r="B11" s="1">
-        <v>1.818287037037037E-2</v>
+      <c r="B11">
+        <f>12*60+35.4</f>
+        <v>755.4</v>
       </c>
       <c r="C11">
         <v>2020</v>
       </c>
       <c r="D11" t="s">
-        <v>12</v>
+        <v>16</v>
       </c>
       <c r="E11">
         <v>52</v>
       </c>
       <c r="F11">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6">
+        <v>1.67</v>
+      </c>
+      <c r="G11" s="1"/>
+    </row>
+    <row r="12" spans="1:7">
       <c r="A12">
+        <v>10000</v>
+      </c>
+      <c r="B12">
+        <f>26*60+11</f>
+        <v>1571</v>
+      </c>
+      <c r="C12">
+        <v>2020</v>
+      </c>
+      <c r="D12" t="s">
+        <v>16</v>
+      </c>
+      <c r="E12">
+        <v>52</v>
+      </c>
+      <c r="F12">
+        <v>1.67</v>
+      </c>
+      <c r="G12" s="1"/>
+    </row>
+    <row r="13" spans="1:7">
+      <c r="A13">
         <v>21097</v>
       </c>
-      <c r="B12" s="3">
-        <v>3.9942129629629626E-2</v>
-      </c>
-      <c r="C12">
+      <c r="B13">
+        <f>57*60+31</f>
+        <v>3451</v>
+      </c>
+      <c r="C13">
         <v>2021</v>
       </c>
-      <c r="D12" t="s">
-        <v>13</v>
-      </c>
-      <c r="E12">
+      <c r="D13" t="s">
+        <v>17</v>
+      </c>
+      <c r="E13">
         <v>56</v>
       </c>
-      <c r="F12">
-        <v>175</v>
-      </c>
-    </row>
-    <row r="13" spans="1:6">
-      <c r="A13">
+      <c r="F13">
+        <v>1.75</v>
+      </c>
+      <c r="G13" s="3"/>
+    </row>
+    <row r="14" spans="1:7">
+      <c r="A14">
         <v>42195</v>
       </c>
-      <c r="B13" s="3">
-        <v>8.4479166666666661E-2</v>
-      </c>
-      <c r="C13">
+      <c r="B14">
+        <f>2*60*60+1*60+39</f>
+        <v>7299</v>
+      </c>
+      <c r="C14">
         <v>2018</v>
       </c>
-      <c r="D13" t="s">
-        <v>14</v>
-      </c>
-      <c r="E13">
+      <c r="D14" t="s">
+        <v>18</v>
+      </c>
+      <c r="E14">
         <v>52</v>
       </c>
-      <c r="F13">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="14" spans="1:6">
-      <c r="B14" s="2"/>
+      <c r="F14">
+        <v>1.67</v>
+      </c>
+      <c r="G14" s="3"/>
+    </row>
+    <row r="15" spans="1:7">
+      <c r="B15" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>